<commit_message>
add test result for N=365 in result.xlsx
</commit_message>
<xml_diff>
--- a/TestResults/result.xlsx
+++ b/TestResults/result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>M \ CPUs</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,6 +34,14 @@
   </si>
   <si>
     <t>Time * CPUs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N=365</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -57,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -359,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K15"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -370,6 +385,11 @@
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
@@ -642,6 +662,232 @@
       </c>
       <c r="E15">
         <v>1.4017500000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1000000</v>
+      </c>
+      <c r="B21">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="C21">
+        <v>25.754999999999999</v>
+      </c>
+      <c r="D21">
+        <v>16.779</v>
+      </c>
+      <c r="E21">
+        <v>12.632</v>
+      </c>
+      <c r="G21">
+        <v>1000000</v>
+      </c>
+      <c r="H21">
+        <f>B21*B$3</f>
+        <v>49.823999999999998</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:I24" si="2">C21*C$3</f>
+        <v>51.51</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ref="J21:J24" si="3">D21*D$3</f>
+        <v>50.337000000000003</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:K24" si="4">E21*E$3</f>
+        <v>50.527999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5000000</v>
+      </c>
+      <c r="B22">
+        <v>247.946</v>
+      </c>
+      <c r="C22">
+        <v>127.39</v>
+      </c>
+      <c r="D22">
+        <v>83.707999999999998</v>
+      </c>
+      <c r="E22">
+        <v>63.932000000000002</v>
+      </c>
+      <c r="G22">
+        <v>5000000</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ref="H22:H24" si="5">B22*B$3</f>
+        <v>247.946</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>254.78</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>251.124</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>255.72800000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10000000</v>
+      </c>
+      <c r="B23">
+        <v>496.32799999999997</v>
+      </c>
+      <c r="C23">
+        <v>253.42400000000001</v>
+      </c>
+      <c r="D23">
+        <v>167.04</v>
+      </c>
+      <c r="E23">
+        <v>130.21299999999999</v>
+      </c>
+      <c r="G23">
+        <v>10000000</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="5"/>
+        <v>496.32799999999997</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>506.84800000000001</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>501.12</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>520.85199999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1000000</v>
+      </c>
+      <c r="B29">
+        <v>1.0855991000000001E-2</v>
+      </c>
+      <c r="C29">
+        <v>1.9014099999999999E-2</v>
+      </c>
+      <c r="D29">
+        <v>1.5882193999999999E-2</v>
+      </c>
+      <c r="E29">
+        <v>6.4672210000000004E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5000000</v>
+      </c>
+      <c r="B30">
+        <v>3.1559880000000002E-3</v>
+      </c>
+      <c r="C30">
+        <v>5.5498170000000003E-3</v>
+      </c>
+      <c r="D30">
+        <v>5.1467099999999997E-3</v>
+      </c>
+      <c r="E30">
+        <v>1.8271439999999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10000000</v>
+      </c>
+      <c r="B31">
+        <v>4.3081700000000001E-4</v>
+      </c>
+      <c r="C31">
+        <v>1.016266E-3</v>
+      </c>
+      <c r="D31">
+        <v>9.7442600000000002E-4</v>
+      </c>
+      <c r="E31">
+        <v>2.4162399999999999E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>